<commit_message>
Calculate d in separate method, tests
</commit_message>
<xml_diff>
--- a/tests/testthat/dyncov_LL_reference.xlsx
+++ b/tests/testthat/dyncov_LL_reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrik/StudentAssi/GIT/CLVTools/tests/testthat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeffr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E628682E-C84B-3843-9486-2D61BCB1A3F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663B6874-35B3-455D-9784-321C1DB5CF9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="500" windowWidth="27640" windowHeight="17500" xr2:uid="{8D303423-B6EF-E442-A975-6C1AD4B476F2}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{8D303423-B6EF-E442-A975-6C1AD4B476F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Walk d" sheetId="3" r:id="rId1"/>
@@ -801,16 +801,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E216C0E4-00F7-514F-B1CA-ABBDD7295FF3}">
   <dimension ref="A5:V54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="2" max="22" width="5.83203125" customWidth="1"/>
+    <col min="2" max="22" width="5.8125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:22" s="34" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" s="34" customFormat="1" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="34" t="s">
         <v>36</v>
       </c>
@@ -824,7 +824,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="27"/>
       <c r="C6" s="28"/>
       <c r="D6" s="28"/>
@@ -847,7 +847,7 @@
       <c r="U6" s="28"/>
       <c r="V6" s="29"/>
     </row>
-    <row r="7" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A7" s="34" t="s">
         <v>37</v>
       </c>
@@ -915,7 +915,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -943,11 +943,13 @@
       <c r="U8" s="30"/>
       <c r="V8" s="30"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="35"/>
+      <c r="B9" s="35">
+        <v>6</v>
+      </c>
       <c r="C9" s="35"/>
       <c r="D9" s="35"/>
       <c r="E9" s="35"/>
@@ -968,11 +970,13 @@
       <c r="T9" s="35"/>
       <c r="U9" s="35"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="35"/>
+      <c r="B10" s="35">
+        <v>6</v>
+      </c>
       <c r="C10" s="35"/>
       <c r="D10" s="35"/>
       <c r="E10" s="35"/>
@@ -993,7 +997,7 @@
       <c r="T10" s="35"/>
       <c r="U10" s="35"/>
     </row>
-    <row r="13" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="34" t="s">
         <v>36</v>
       </c>
@@ -1025,7 +1029,7 @@
       <c r="U13" s="34"/>
       <c r="V13" s="34"/>
     </row>
-    <row r="14" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="27"/>
       <c r="C14" s="28"/>
       <c r="D14" s="28"/>
@@ -1048,7 +1052,7 @@
       <c r="U14" s="28"/>
       <c r="V14" s="29"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A15" s="34" t="s">
         <v>37</v>
       </c>
@@ -1116,7 +1120,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -1143,11 +1147,13 @@
       <c r="U16" s="30"/>
       <c r="V16" s="30"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="35"/>
+      <c r="B17" s="35">
+        <v>5</v>
+      </c>
       <c r="C17" s="35"/>
       <c r="D17" s="35"/>
       <c r="E17" s="35"/>
@@ -1168,11 +1174,13 @@
       <c r="T17" s="35"/>
       <c r="U17" s="35"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="35"/>
+      <c r="B18" s="35">
+        <v>5</v>
+      </c>
       <c r="C18" s="35"/>
       <c r="D18" s="35"/>
       <c r="E18" s="35"/>
@@ -1193,7 +1201,7 @@
       <c r="T18" s="35"/>
       <c r="U18" s="35"/>
     </row>
-    <row r="21" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="34" t="s">
         <v>36</v>
       </c>
@@ -1225,7 +1233,7 @@
       <c r="U21" s="34"/>
       <c r="V21" s="34"/>
     </row>
-    <row r="22" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="27"/>
       <c r="C22" s="28"/>
       <c r="D22" s="28"/>
@@ -1248,7 +1256,7 @@
       <c r="U22" s="28"/>
       <c r="V22" s="29"/>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A23" s="34" t="s">
         <v>37</v>
       </c>
@@ -1316,7 +1324,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1343,11 +1351,13 @@
       <c r="U24" s="30"/>
       <c r="V24" s="30"/>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="35"/>
+      <c r="B25" s="35">
+        <v>4</v>
+      </c>
       <c r="C25" s="35"/>
       <c r="D25" s="35"/>
       <c r="E25" s="35"/>
@@ -1368,11 +1378,13 @@
       <c r="T25" s="35"/>
       <c r="U25" s="35"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="35"/>
+      <c r="B26" s="35">
+        <v>4</v>
+      </c>
       <c r="C26" s="35"/>
       <c r="D26" s="35"/>
       <c r="E26" s="35"/>
@@ -1393,7 +1405,7 @@
       <c r="T26" s="35"/>
       <c r="U26" s="35"/>
     </row>
-    <row r="28" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="34" t="s">
         <v>36</v>
       </c>
@@ -1425,7 +1437,7 @@
       <c r="U28" s="34"/>
       <c r="V28" s="34"/>
     </row>
-    <row r="29" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" s="27"/>
       <c r="C29" s="28"/>
       <c r="D29" s="28"/>
@@ -1448,7 +1460,7 @@
       <c r="U29" s="28"/>
       <c r="V29" s="29"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A30" s="34" t="s">
         <v>37</v>
       </c>
@@ -1516,7 +1528,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1542,11 +1554,13 @@
       <c r="U31" s="30"/>
       <c r="V31" s="30"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="35"/>
+      <c r="B32" s="35">
+        <v>3</v>
+      </c>
       <c r="C32" s="35"/>
       <c r="D32" s="35"/>
       <c r="E32" s="35"/>
@@ -1567,11 +1581,13 @@
       <c r="T32" s="35"/>
       <c r="U32" s="35"/>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="35"/>
+      <c r="B33" s="35">
+        <v>3</v>
+      </c>
       <c r="C33" s="35"/>
       <c r="D33" s="35"/>
       <c r="E33" s="35"/>
@@ -1592,7 +1608,7 @@
       <c r="T33" s="35"/>
       <c r="U33" s="35"/>
     </row>
-    <row r="35" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="34" t="s">
         <v>36</v>
       </c>
@@ -1624,7 +1640,7 @@
       <c r="U35" s="34"/>
       <c r="V35" s="34"/>
     </row>
-    <row r="36" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B36" s="27"/>
       <c r="C36" s="28"/>
       <c r="D36" s="28"/>
@@ -1647,7 +1663,7 @@
       <c r="U36" s="28"/>
       <c r="V36" s="29"/>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A37" s="34" t="s">
         <v>37</v>
       </c>
@@ -1715,7 +1731,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -1741,11 +1757,13 @@
       <c r="U38" s="30"/>
       <c r="V38" s="30"/>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="35"/>
+      <c r="B39" s="35">
+        <v>2</v>
+      </c>
       <c r="C39" s="35"/>
       <c r="D39" s="35"/>
       <c r="E39" s="35"/>
@@ -1766,11 +1784,13 @@
       <c r="T39" s="35"/>
       <c r="U39" s="35"/>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="35"/>
+      <c r="B40" s="35">
+        <v>2</v>
+      </c>
       <c r="C40" s="35"/>
       <c r="D40" s="35"/>
       <c r="E40" s="35"/>
@@ -1791,7 +1811,7 @@
       <c r="T40" s="35"/>
       <c r="U40" s="35"/>
     </row>
-    <row r="42" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="34" t="s">
         <v>36</v>
       </c>
@@ -1823,7 +1843,7 @@
       <c r="U42" s="34"/>
       <c r="V42" s="34"/>
     </row>
-    <row r="43" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B43" s="27"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
@@ -1846,7 +1866,7 @@
       <c r="U43" s="28"/>
       <c r="V43" s="29"/>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A44" s="34" t="s">
         <v>37</v>
       </c>
@@ -1914,7 +1934,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
         <v>35</v>
       </c>
@@ -1940,11 +1960,13 @@
       <c r="U45" s="30"/>
       <c r="V45" s="30"/>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A46" t="s">
         <v>5</v>
       </c>
-      <c r="B46" s="35"/>
+      <c r="B46" s="35">
+        <v>1</v>
+      </c>
       <c r="C46" s="35"/>
       <c r="D46" s="35"/>
       <c r="E46" s="35"/>
@@ -1965,11 +1987,13 @@
       <c r="T46" s="35"/>
       <c r="U46" s="35"/>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A47" t="s">
         <v>4</v>
       </c>
-      <c r="B47" s="35"/>
+      <c r="B47" s="35">
+        <v>1</v>
+      </c>
       <c r="C47" s="35"/>
       <c r="D47" s="35"/>
       <c r="E47" s="35"/>
@@ -1990,7 +2014,7 @@
       <c r="T47" s="35"/>
       <c r="U47" s="35"/>
     </row>
-    <row r="49" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="34" t="s">
         <v>36</v>
       </c>
@@ -2022,7 +2046,7 @@
       <c r="U49" s="34"/>
       <c r="V49" s="34"/>
     </row>
-    <row r="50" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B50" s="27"/>
       <c r="C50" s="28"/>
       <c r="D50" s="28"/>
@@ -2045,7 +2069,7 @@
       <c r="U50" s="28"/>
       <c r="V50" s="29"/>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A51" s="34" t="s">
         <v>37</v>
       </c>
@@ -2113,7 +2137,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A52" t="s">
         <v>35</v>
       </c>
@@ -2139,11 +2163,13 @@
       <c r="U52" s="30"/>
       <c r="V52" s="30"/>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A53" t="s">
         <v>5</v>
       </c>
-      <c r="B53" s="35"/>
+      <c r="B53" s="35">
+        <v>0</v>
+      </c>
       <c r="C53" s="35"/>
       <c r="D53" s="35"/>
       <c r="E53" s="35"/>
@@ -2165,11 +2191,13 @@
       <c r="U53" s="35"/>
       <c r="V53" s="35"/>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A54" t="s">
         <v>4</v>
       </c>
-      <c r="B54" s="35"/>
+      <c r="B54" s="35">
+        <v>0</v>
+      </c>
       <c r="C54" s="35"/>
       <c r="D54" s="35"/>
       <c r="E54" s="35"/>
@@ -2202,18 +2230,18 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="2" max="2" width="6.5" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.8125" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="6.5" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" customWidth="1"/>
+    <col min="8" max="8" width="11.1875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2236,7 +2264,7 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2" s="1"/>
       <c r="B2" s="1">
         <v>4</v>
@@ -2257,7 +2285,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2268,7 +2296,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A4" s="20" t="s">
         <v>23</v>
       </c>
@@ -2281,7 +2309,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A5" s="20" t="s">
         <v>22</v>
       </c>
@@ -2294,7 +2322,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2305,7 +2333,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
       <c r="B7" s="4" t="s">
         <v>15</v>
       </c>
@@ -2317,7 +2345,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A8" s="1"/>
       <c r="B8" s="2">
         <v>0.123</v>
@@ -2340,7 +2368,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A9" s="1"/>
       <c r="B9" s="8" t="s">
         <v>1</v>
@@ -2355,7 +2383,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>9</v>
@@ -2370,7 +2398,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -2388,7 +2416,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2406,7 +2434,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2424,7 +2452,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -2442,7 +2470,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -2460,7 +2488,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -2472,13 +2500,13 @@
         <v>-25.388549999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.5">
       <c r="B18" s="4" t="s">
         <v>15</v>
       </c>
@@ -2490,7 +2518,7 @@
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A19" s="1"/>
       <c r="B19" s="2">
         <v>0.123</v>
@@ -2509,7 +2537,7 @@
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A20" s="1"/>
       <c r="B20" s="8" t="s">
         <v>1</v>
@@ -2524,7 +2552,7 @@
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
         <v>9</v>
@@ -2539,7 +2567,7 @@
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -2557,7 +2585,7 @@
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
@@ -2575,7 +2603,7 @@
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A24" s="1" t="s">
         <v>11</v>
       </c>
@@ -2593,7 +2621,7 @@
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A25" s="1" t="s">
         <v>12</v>
       </c>
@@ -2611,7 +2639,7 @@
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A26" s="1"/>
       <c r="B26" s="3"/>
       <c r="C26" s="1"/>
@@ -2622,7 +2650,7 @@
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.5">
       <c r="B27" s="4" t="s">
         <v>15</v>
       </c>
@@ -2634,7 +2662,7 @@
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A28" s="1"/>
       <c r="B28" s="2">
         <v>0.123</v>
@@ -2653,7 +2681,7 @@
       </c>
       <c r="I28" s="7"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A29" s="1"/>
       <c r="B29" s="8" t="s">
         <v>1</v>
@@ -2668,7 +2696,7 @@
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
         <v>9</v>
@@ -2683,7 +2711,7 @@
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A31" s="1" t="s">
         <v>7</v>
       </c>
@@ -2696,7 +2724,7 @@
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A32" s="1" t="s">
         <v>10</v>
       </c>
@@ -2709,7 +2737,7 @@
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A33" s="1" t="s">
         <v>11</v>
       </c>
@@ -2722,7 +2750,7 @@
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A34" s="1"/>
       <c r="B34" s="3"/>
       <c r="C34" s="1"/>
@@ -2733,7 +2761,7 @@
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.5">
       <c r="B35" s="4" t="s">
         <v>15</v>
       </c>
@@ -2745,7 +2773,7 @@
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A36" s="1"/>
       <c r="B36" s="2">
         <v>0.123</v>
@@ -2760,7 +2788,7 @@
       <c r="H36" s="7"/>
       <c r="I36" s="7"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A37" s="1"/>
       <c r="B37" s="8" t="s">
         <v>1</v>
@@ -2775,7 +2803,7 @@
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
         <v>9</v>
@@ -2790,7 +2818,7 @@
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A39" s="1" t="s">
         <v>7</v>
       </c>
@@ -2806,7 +2834,7 @@
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A40" s="1" t="s">
         <v>10</v>
       </c>
@@ -2822,7 +2850,7 @@
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A41" s="1"/>
       <c r="B41" s="3"/>
       <c r="C41" s="1"/>
@@ -2833,7 +2861,7 @@
       <c r="H41" s="7"/>
       <c r="I41" s="7"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.5">
       <c r="B42" s="4" t="s">
         <v>15</v>
       </c>
@@ -2844,7 +2872,7 @@
       <c r="H42" s="7"/>
       <c r="I42" s="7"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A43" s="1"/>
       <c r="B43" s="2">
         <v>0.123</v>
@@ -2852,7 +2880,7 @@
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A44" s="1"/>
       <c r="B44" s="8" t="s">
         <v>16</v>
@@ -2860,7 +2888,7 @@
       <c r="C44" s="1"/>
       <c r="D44" s="5"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
         <v>9</v>
@@ -2870,7 +2898,7 @@
       </c>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A46" s="1" t="s">
         <v>7</v>
       </c>
@@ -2881,13 +2909,13 @@
       </c>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A49" s="23" t="s">
         <v>28</v>
       </c>
@@ -2906,15 +2934,15 @@
       <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" customWidth="1"/>
-    <col min="4" max="8" width="7.6640625" customWidth="1"/>
-    <col min="11" max="13" width="5.1640625" customWidth="1"/>
+    <col min="3" max="3" width="18.1875" customWidth="1"/>
+    <col min="4" max="8" width="7.6875" customWidth="1"/>
+    <col min="11" max="13" width="5.1875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2931,7 +2959,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A2" s="1"/>
       <c r="B2" s="1">
         <v>4</v>
@@ -2946,35 +2974,35 @@
         <v>0.85399999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A4" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A5" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A6" s="9" t="s">
         <v>22</v>
       </c>
       <c r="J6" s="11"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A7" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B9" s="17" t="s">
         <v>18</v>
       </c>
@@ -2995,7 +3023,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B10" s="15" t="s">
         <v>17</v>
       </c>
@@ -3009,7 +3037,7 @@
       <c r="K10" s="18"/>
       <c r="L10" s="18"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="18" t="s">
@@ -3021,7 +3049,7 @@
       <c r="K11" s="18"/>
       <c r="L11" s="18"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -3037,7 +3065,7 @@
       <c r="K12" s="16"/>
       <c r="L12" s="16"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -3061,7 +3089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B15" s="17" t="s">
         <v>18</v>
       </c>
@@ -3071,7 +3099,7 @@
       </c>
       <c r="E15" s="10"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B16" s="15" t="s">
         <v>17</v>
       </c>
@@ -3083,7 +3111,7 @@
         <v>0.23400000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="18" t="s">
@@ -3093,7 +3121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B18" t="s">
         <v>9</v>
       </c>
@@ -3105,7 +3133,7 @@
       </c>
       <c r="E18" s="16"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -3129,7 +3157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -3154,7 +3182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B22" s="17" t="s">
         <v>18</v>
       </c>
@@ -3165,7 +3193,7 @@
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B23" s="15" t="s">
         <v>17</v>
       </c>
@@ -3180,7 +3208,7 @@
         <v>0.34499999999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="18" t="s">
@@ -3191,7 +3219,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B25" t="s">
         <v>9</v>
       </c>
@@ -3204,7 +3232,7 @@
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -3228,7 +3256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -3253,7 +3281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -3278,7 +3306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B30" s="17" t="s">
         <v>18</v>
       </c>
@@ -3290,7 +3318,7 @@
       <c r="F30" s="10"/>
       <c r="G30" s="11"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B31" s="15" t="s">
         <v>17</v>
       </c>
@@ -3308,7 +3336,7 @@
         <v>0.45600000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
       <c r="D32" s="18" t="s">
@@ -3320,7 +3348,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B33" t="s">
         <v>9</v>
       </c>
@@ -3334,7 +3362,7 @@
       <c r="F33" s="16"/>
       <c r="G33" s="16"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -3358,7 +3386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -3383,7 +3411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -3408,7 +3436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -3433,7 +3461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B40" s="17" t="s">
         <v>18</v>
       </c>
@@ -3443,7 +3471,7 @@
       </c>
       <c r="E40" s="10"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B41" s="12">
         <v>1.9870000000000001</v>
       </c>
@@ -3453,7 +3481,7 @@
       </c>
       <c r="E41" s="18"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B42" s="21">
         <v>0</v>
       </c>
@@ -3463,7 +3491,7 @@
       </c>
       <c r="E42" s="18"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B43" t="s">
         <v>9</v>
       </c>
@@ -3475,7 +3503,7 @@
       </c>
       <c r="E43" s="16"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -3503,7 +3531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B46" s="17" t="s">
         <v>18</v>
       </c>
@@ -3512,7 +3540,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B47" s="12">
         <v>1.9870000000000001</v>
       </c>
@@ -3524,7 +3552,7 @@
         <v>0.23400000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B48" s="21">
         <v>0</v>
       </c>
@@ -3536,7 +3564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B49" t="s">
         <v>9</v>
       </c>
@@ -3547,7 +3575,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -3572,7 +3600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A51" t="s">
         <v>10</v>
       </c>
@@ -3597,7 +3625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B53" s="17" t="s">
         <v>18</v>
       </c>
@@ -3606,7 +3634,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B54" s="12">
         <v>1.9870000000000001</v>
       </c>
@@ -3621,7 +3649,7 @@
         <v>0.34499999999999997</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B55" s="21">
         <v>0</v>
       </c>
@@ -3634,7 +3662,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B56" t="s">
         <v>9</v>
       </c>
@@ -3645,7 +3673,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A57" t="s">
         <v>7</v>
       </c>
@@ -3673,7 +3701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A58" t="s">
         <v>10</v>
       </c>
@@ -3698,7 +3726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A59" t="s">
         <v>11</v>
       </c>
@@ -3723,7 +3751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B61" s="17" t="s">
         <v>18</v>
       </c>
@@ -3732,7 +3760,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B62" s="12">
         <v>1.9870000000000001</v>
       </c>
@@ -3750,7 +3778,7 @@
         <v>0.45600000000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B63" s="21">
         <v>0</v>
       </c>
@@ -3764,7 +3792,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B64" t="s">
         <v>9</v>
       </c>
@@ -3775,7 +3803,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A65" t="s">
         <v>7</v>
       </c>
@@ -3803,7 +3831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A66" t="s">
         <v>10</v>
       </c>
@@ -3828,7 +3856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A67" t="s">
         <v>11</v>
       </c>
@@ -3853,7 +3881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A68" t="s">
         <v>12</v>
       </c>
@@ -3878,7 +3906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B70" s="17" t="s">
         <v>18</v>
       </c>
@@ -3887,7 +3915,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B71" s="12">
         <v>1.9870000000000001</v>
       </c>
@@ -3900,7 +3928,7 @@
       <c r="F71" s="18"/>
       <c r="G71" s="18"/>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B72" s="21">
         <v>0</v>
       </c>
@@ -3911,7 +3939,7 @@
       <c r="F72" s="18"/>
       <c r="G72" s="18"/>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B73" t="s">
         <v>9</v>
       </c>
@@ -3922,7 +3950,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A74" t="s">
         <v>7</v>
       </c>
@@ -3947,7 +3975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B76" s="17" t="s">
         <v>18</v>
       </c>
@@ -3956,7 +3984,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B77" s="12">
         <v>1.9870000000000001</v>
       </c>
@@ -3971,7 +3999,7 @@
       </c>
       <c r="G77" s="18"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B78" s="21">
         <v>0</v>
       </c>
@@ -3984,7 +4012,7 @@
       </c>
       <c r="G78" s="18"/>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B79" t="s">
         <v>9</v>
       </c>
@@ -3995,7 +4023,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A80" t="s">
         <v>7</v>
       </c>
@@ -4020,7 +4048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A81" t="s">
         <v>10</v>
       </c>
@@ -4045,7 +4073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B83" s="17" t="s">
         <v>18</v>
       </c>
@@ -4054,7 +4082,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B84" s="12">
         <v>1.9870000000000001</v>
       </c>
@@ -4071,7 +4099,7 @@
         <v>0.34499999999999997</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B85" s="21">
         <v>0</v>
       </c>
@@ -4084,7 +4112,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B86" t="s">
         <v>9</v>
       </c>
@@ -4095,7 +4123,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A87" t="s">
         <v>7</v>
       </c>
@@ -4123,7 +4151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A88" t="s">
         <v>10</v>
       </c>
@@ -4148,7 +4176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A89" t="s">
         <v>11</v>
       </c>
@@ -4173,7 +4201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B91" s="17" t="s">
         <v>18</v>
       </c>
@@ -4182,7 +4210,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B92" s="12">
         <v>1.9870000000000001</v>
       </c>
@@ -4202,7 +4230,7 @@
         <v>0.45600000000000002</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B93" s="21">
         <v>0</v>
       </c>
@@ -4216,7 +4244,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B94" t="s">
         <v>9</v>
       </c>
@@ -4227,7 +4255,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A95" t="s">
         <v>7</v>
       </c>
@@ -4255,7 +4283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A96" t="s">
         <v>10</v>
       </c>
@@ -4280,7 +4308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A97" t="s">
         <v>11</v>
       </c>
@@ -4305,7 +4333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A98" t="s">
         <v>12</v>
       </c>

</xml_diff>